<commit_message>
sending email with outlook
</commit_message>
<xml_diff>
--- a/REFrameworkTest/reqests.xlsx
+++ b/REFrameworkTest/reqests.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -125,16 +126,27 @@
   </si>
   <si>
     <t>success: Single Result</t>
+  </si>
+  <si>
+    <t>boogh313@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,13 +169,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +508,9 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -519,6 +537,9 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
@@ -545,6 +566,9 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
@@ -571,6 +595,9 @@
       <c r="B5" t="s">
         <v>21</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
@@ -597,6 +624,9 @@
       <c r="B6" t="s">
         <v>21</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
@@ -623,6 +653,9 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
@@ -649,6 +682,9 @@
       <c r="B8" t="s">
         <v>25</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
@@ -675,6 +711,9 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
@@ -701,6 +740,9 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
@@ -724,6 +766,9 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
@@ -747,6 +792,9 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -764,12 +812,155 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3:C12" r:id="rId2" display="boogh313@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>7845</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>5011</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3:C4" r:id="rId2" display="boogh313@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>

</xml_diff>